<commit_message>
compiled all probabilities from mlogit and clogit and added to formatted excel
</commit_message>
<xml_diff>
--- a/output/pooled_marg_probs_formatted.xlsx
+++ b/output/pooled_marg_probs_formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gclawson/Desktop/PangaWatch/DRCE-Analysis/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FE7535-9C13-7449-9966-F5F56EB2D557}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD8EDC2-89C1-E84C-B15C-96679D308058}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15600" xr2:uid="{907326D8-DECD-9A42-B268-CE0ADB5B6D89}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>mlogit</t>
   </si>
@@ -73,6 +73,30 @@
   </si>
   <si>
     <t>formula</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>info</t>
+  </si>
+  <si>
+    <t>sos</t>
+  </si>
+  <si>
+    <t>own</t>
+  </si>
+  <si>
+    <t>lin_pred_probs</t>
+  </si>
+  <si>
+    <t>probs_form</t>
+  </si>
+  <si>
+    <t>predict_probs</t>
+  </si>
+  <si>
+    <t>fitted_probs</t>
   </si>
 </sst>
 </file>
@@ -116,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,27 +460,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A888EF95-3E46-7141-ADC8-C6D5DF05DB73}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,7 +499,7 @@
       <c r="K1" s="3"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -504,7 +532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -539,7 +567,7 @@
         <v>6.1303754513629398</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -574,7 +602,7 @@
         <v>6.8038606823972296</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -609,7 +637,7 @@
         <v>6.1303754513629398</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -622,7 +650,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -637,7 +665,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>1</v>
@@ -670,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -705,7 +733,7 @@
         <v>21.1295679003887</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -740,7 +768,7 @@
         <v>22.0163893899512</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -773,6 +801,711 @@
       </c>
       <c r="K11" s="3">
         <v>6.1303754513629496</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.82662101815191E-2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.39052830927507098</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.10642841372506801</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0.39052830927507098</v>
+      </c>
+      <c r="N16" s="4">
+        <v>9.8958683541390105E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.97881384301214902</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.97207899070180603</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.86615666415119297</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0.97207899070180603</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0.85647316833813802</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.50684957566686795</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.74510111841111404</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.352057188605996</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.74510111841111404</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0.33378760950229303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.78751981704009599</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.92091614808901101</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0.68399627242046401</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0.92091614808901101</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0.66621239049770697</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4">
+        <v>8.9224763811823704E-2</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.156743321243619</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0.14632047016760999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4">
+        <v>7.9848876956412906E-2</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.773279068321995</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.38799649457985502</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0.773279068321995</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0.36892379232842698</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.92368365956711895</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.97489434681082499</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0.878315499273707</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.97489434681082499</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0.86937902768754505</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.13555710603683399</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.46711684248344898</v>
+      </c>
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0.14010904380681799</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0.46711684248344898</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0.13062097231245501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.88001671440332996</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.97544025996607597</v>
+      </c>
+      <c r="H24">
+        <v>9</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0.88070450306884795</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.97544025996607597</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0.87191789416390197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.13331229176992701</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.42229254948766398</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0.11962026086619799</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0.42229254948766398</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.111340019664445</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.91077523618817602</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.91077523618817602</v>
+      </c>
+      <c r="H26">
+        <v>11</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0.65486098514730595</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0.91077523618817602</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0.63630927443862595</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.88375662740906002</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.97146054934477599</v>
+      </c>
+      <c r="H27">
+        <v>12</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0.86352147292297299</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0.97146054934477599</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0.85367952983239004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.39329315020231598</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.88181887181914498</v>
+      </c>
+      <c r="H28">
+        <v>13</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28" s="4">
+        <v>0.581055157838126</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0.88181887181914498</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0.56119457598552802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.53275397131476099</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.89487096187632698</v>
+      </c>
+      <c r="H29">
+        <v>14</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29" s="4">
+        <v>0.61273638784453799</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0.89487096187632698</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0.59332654038341803</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.52141123392793198</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.76930229453210097</v>
+      </c>
+      <c r="H30">
+        <v>15</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0.38265693131505801</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.76930229453209997</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0.363690725561374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.17877720027876001</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.74935915417856103</v>
+      </c>
+      <c r="H31">
+        <v>16</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0.357216835159824</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0.74935915417856103</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0.33881951504832802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>